<commit_message>
Update ngày kế hoạch
</commit_message>
<xml_diff>
--- a/Kế Hoạch.xlsx
+++ b/Kế Hoạch.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>Danh sách kế hoạch</t>
   </si>
@@ -168,16 +168,7 @@
     <t>30/9/2020</t>
   </si>
   <si>
-    <t>20/12/2020</t>
-  </si>
-  <si>
-    <t>24/12/2020</t>
-  </si>
-  <si>
     <t>19/12/2020</t>
-  </si>
-  <si>
-    <t>18/12/2020</t>
   </si>
   <si>
     <t>13/9/2020</t>
@@ -240,6 +231,9 @@
   </si>
   <si>
     <t xml:space="preserve">ChatBot trả lời </t>
+  </si>
+  <si>
+    <t>13/12/2020</t>
   </si>
 </sst>
 </file>
@@ -779,7 +773,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -834,7 +828,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61DD5472-8C3B-423D-B078-5E3B4DC3F79D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61DD5472-8C3B-423D-B078-5E3B4DC3F79D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1168,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:UP86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1503,7 +1497,7 @@
         <v>44083</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -1528,7 +1522,7 @@
         <v>42</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
@@ -1602,10 +1596,10 @@
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -4592,7 +4586,7 @@
         <v>43961</v>
       </c>
       <c r="F28" s="48" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G28" s="48"/>
       <c r="I28" s="44"/>
@@ -5723,7 +5717,7 @@
         <v>4.2</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -6291,7 +6285,7 @@
         <v>4.3</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -6314,7 +6308,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -6337,7 +6331,7 @@
         <v>4.5</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -6425,7 +6419,7 @@
         <v>43992</v>
       </c>
       <c r="F37" s="25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G37" s="25"/>
       <c r="H37" s="25"/>
@@ -6444,7 +6438,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C38" s="32"/>
       <c r="D38" s="32"/>
@@ -6458,7 +6452,7 @@
         <v>5.2</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -6556,7 +6550,7 @@
         <v>44114</v>
       </c>
       <c r="F44" s="27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G44" s="27"/>
       <c r="H44" s="27"/>
@@ -6575,7 +6569,7 @@
         <v>6.1</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
@@ -6770,8 +6764,8 @@
       </c>
       <c r="C54" s="56"/>
       <c r="D54" s="56"/>
-      <c r="E54" s="57">
-        <v>43902</v>
+      <c r="E54" s="57" t="s">
+        <v>56</v>
       </c>
       <c r="F54" s="57">
         <v>43963</v>
@@ -6840,10 +6834,10 @@
       <c r="C57" s="56"/>
       <c r="D57" s="56"/>
       <c r="E57" s="57">
-        <v>43994</v>
+        <v>43842</v>
       </c>
       <c r="F57" s="57">
-        <v>44147</v>
+        <v>43963</v>
       </c>
       <c r="G57" s="56"/>
       <c r="H57" s="55"/>
@@ -6867,10 +6861,10 @@
       <c r="C58" s="56"/>
       <c r="D58" s="56"/>
       <c r="E58" s="57">
-        <v>43994</v>
+        <v>43842</v>
       </c>
       <c r="F58" s="57">
-        <v>44147</v>
+        <v>43963</v>
       </c>
       <c r="G58" s="56"/>
       <c r="H58" s="55"/>
@@ -6955,10 +6949,10 @@
       <c r="C62" s="19"/>
       <c r="D62" s="19"/>
       <c r="E62" s="20">
+        <v>43994</v>
+      </c>
+      <c r="F62" s="20">
         <v>44177</v>
-      </c>
-      <c r="F62" s="20" t="s">
-        <v>51</v>
       </c>
       <c r="G62" s="19"/>
       <c r="H62" s="18"/>
@@ -6982,10 +6976,10 @@
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
       <c r="E63" s="20">
+        <v>44024</v>
+      </c>
+      <c r="F63" s="20">
         <v>44177</v>
-      </c>
-      <c r="F63" s="20" t="s">
-        <v>51</v>
       </c>
       <c r="G63" s="19"/>
       <c r="H63" s="18"/>
@@ -7009,10 +7003,10 @@
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
       <c r="E64" s="20" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G64" s="19"/>
       <c r="H64" s="18"/>
@@ -7036,10 +7030,10 @@
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
       <c r="E65" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F65" s="20" t="s">
         <v>48</v>
-      </c>
-      <c r="F65" s="20" t="s">
-        <v>49</v>
       </c>
       <c r="G65" s="19"/>
       <c r="H65" s="18"/>

</xml_diff>

<commit_message>
Update khảo sát 4 website
</commit_message>
<xml_diff>
--- a/Kế Hoạch.xlsx
+++ b/Kế Hoạch.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>Danh sách kế hoạch</t>
   </si>
@@ -748,10 +748,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -788,7 +788,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -843,7 +843,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61DD5472-8C3B-423D-B078-5E3B4DC3F79D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61DD5472-8C3B-423D-B078-5E3B4DC3F79D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:UP88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1307,7 +1307,7 @@
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" s="12" customFormat="1">
-      <c r="A5" s="68"/>
+      <c r="A5" s="67"/>
       <c r="B5" s="18" t="s">
         <v>11</v>
       </c>
@@ -1338,7 +1338,7 @@
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" s="12" customFormat="1">
-      <c r="A6" s="68"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="18" t="s">
         <v>62</v>
       </c>
@@ -1355,7 +1355,9 @@
       <c r="G6" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="H6" s="20"/>
+      <c r="H6" s="20" t="s">
+        <v>44</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1367,7 +1369,7 @@
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" s="12" customFormat="1">
-      <c r="A7" s="67"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="18" t="s">
         <v>63</v>
       </c>
@@ -1384,7 +1386,9 @@
       <c r="G7" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="20"/>
+      <c r="H7" s="20" t="s">
+        <v>44</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1585,7 +1589,7 @@
       <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17" s="12" customFormat="1">
-      <c r="A15" s="68"/>
+      <c r="A15" s="67"/>
       <c r="B15" s="18" t="s">
         <v>16</v>
       </c>
@@ -1610,7 +1614,7 @@
       <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:17" s="12" customFormat="1">
-      <c r="A16" s="68"/>
+      <c r="A16" s="67"/>
       <c r="B16" s="18" t="s">
         <v>22</v>
       </c>
@@ -1635,7 +1639,7 @@
       <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:562" s="12" customFormat="1">
-      <c r="A17" s="67"/>
+      <c r="A17" s="68"/>
       <c r="B17" s="18" t="s">
         <v>39</v>
       </c>
@@ -1687,7 +1691,7 @@
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:562" s="12" customFormat="1">
-      <c r="A19" s="67"/>
+      <c r="A19" s="68"/>
       <c r="B19" s="18" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Cập nhật kế hoạch thực hiện
</commit_message>
<xml_diff>
--- a/Kế Hoạch.xlsx
+++ b/Kế Hoạch.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
   <si>
     <t>Danh sách kế hoạch</t>
   </si>
@@ -133,12 +133,6 @@
     <t>Làm PowerPoint</t>
   </si>
   <si>
-    <t>In báo cáo</t>
-  </si>
-  <si>
-    <t>Kiểm tra chính tả</t>
-  </si>
-  <si>
     <t>Vẽ sequence diagram mô tả luồng hoạt động</t>
   </si>
   <si>
@@ -249,6 +243,17 @@
   </si>
   <si>
     <t>21/9/2020</t>
+  </si>
+  <si>
+    <t>In báo cáo
+Kiểm tra chính tả</t>
+  </si>
+  <si>
+    <t>14/12/2020</t>
+  </si>
+  <si>
+    <t>Nộp lại cho giáo viên hướng dẫn
+Sau đó hoàn chỉnh báo cáo</t>
   </si>
 </sst>
 </file>
@@ -788,7 +793,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -843,7 +848,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61DD5472-8C3B-423D-B078-5E3B4DC3F79D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61DD5472-8C3B-423D-B078-5E3B4DC3F79D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1177,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:UP88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1340,23 +1345,23 @@
     <row r="6" spans="1:17" s="12" customFormat="1">
       <c r="A6" s="67"/>
       <c r="B6" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>66</v>
-      </c>
       <c r="H6" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1371,23 +1376,23 @@
     <row r="7" spans="1:17" s="12" customFormat="1">
       <c r="A7" s="68"/>
       <c r="B7" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>66</v>
-      </c>
       <c r="H7" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1421,9 +1426,7 @@
       <c r="G8" s="20">
         <v>43991</v>
       </c>
-      <c r="H8" s="20">
-        <v>43960</v>
-      </c>
+      <c r="H8" s="20"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1574,7 +1577,7 @@
         <v>44083</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
@@ -1596,10 +1599,10 @@
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -1621,10 +1624,10 @@
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -1641,15 +1644,15 @@
     <row r="17" spans="1:562" s="12" customFormat="1">
       <c r="A17" s="68"/>
       <c r="B17" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -1673,10 +1676,10 @@
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
@@ -1698,7 +1701,7 @@
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
       <c r="E19" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F19" s="20">
         <v>43840</v>
@@ -1725,7 +1728,7 @@
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F20" s="20">
         <v>43840</v>
@@ -4045,7 +4048,7 @@
         <v>3.1</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
@@ -4663,7 +4666,7 @@
         <v>43961</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G30" s="48"/>
       <c r="I30" s="44"/>
@@ -5226,7 +5229,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -5794,7 +5797,7 @@
         <v>4.2</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -6362,7 +6365,7 @@
         <v>4.3</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -6385,7 +6388,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
@@ -6408,7 +6411,7 @@
         <v>4.5</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -6496,7 +6499,7 @@
         <v>43992</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G39" s="25"/>
       <c r="H39" s="25"/>
@@ -6515,7 +6518,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C40" s="32"/>
       <c r="D40" s="32"/>
@@ -6529,7 +6532,7 @@
         <v>5.2</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
@@ -6627,7 +6630,7 @@
         <v>44114</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G46" s="27"/>
       <c r="H46" s="27"/>
@@ -6646,7 +6649,7 @@
         <v>6.1</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
@@ -6842,7 +6845,7 @@
       <c r="C56" s="56"/>
       <c r="D56" s="56"/>
       <c r="E56" s="57" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F56" s="57">
         <v>43963</v>
@@ -7070,20 +7073,20 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="1:17" s="12" customFormat="1">
+    <row r="66" spans="1:17" s="12" customFormat="1" ht="30">
       <c r="A66" s="21">
         <v>9.3000000000000007</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
       <c r="E66" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="G66" s="19"/>
       <c r="H66" s="18"/>
@@ -7097,20 +7100,20 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="1:17" s="12" customFormat="1">
+    <row r="67" spans="1:17" s="12" customFormat="1" ht="30">
       <c r="A67" s="21">
         <v>9.4</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="19"/>
       <c r="E67" s="20" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G67" s="19"/>
       <c r="H67" s="18"/>

</xml_diff>

<commit_message>
Update ngày vẽ uml
</commit_message>
<xml_diff>
--- a/Kế Hoạch.xlsx
+++ b/Kế Hoạch.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>Danh sách kế hoạch</t>
   </si>
@@ -254,6 +254,9 @@
   <si>
     <t>Nộp lại cho giáo viên hướng dẫn
 Sau đó hoàn chỉnh báo cáo</t>
+  </si>
+  <si>
+    <t>26/9/2020</t>
   </si>
 </sst>
 </file>
@@ -793,7 +796,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -848,7 +851,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61DD5472-8C3B-423D-B078-5E3B4DC3F79D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61DD5472-8C3B-423D-B078-5E3B4DC3F79D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1182,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:UP88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1579,7 +1582,9 @@
       <c r="F14" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="20"/>
+      <c r="G14" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="H14" s="20"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1604,7 +1609,9 @@
       <c r="F15" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="20"/>
+      <c r="G15" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="H15" s="20"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>

</xml_diff>

<commit_message>
Nghiệp vụ website cơ bản
</commit_message>
<xml_diff>
--- a/Kế Hoạch.xlsx
+++ b/Kế Hoạch.xlsx
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Vẽ erd từ lượt đồ use case</t>
-  </si>
-  <si>
-    <t>Vẽ mẫu các trang mình cần có trên figma</t>
   </si>
   <si>
     <t>Liệt kê các trang cần có</t>
@@ -257,6 +254,10 @@
   </si>
   <si>
     <t>26/9/2020</t>
+  </si>
+  <si>
+    <t>Vẽ mẫu các trang mình cần có trên figma
++Dùng  template thay thế</t>
   </si>
 </sst>
 </file>
@@ -796,7 +797,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -851,7 +852,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61DD5472-8C3B-423D-B078-5E3B4DC3F79D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61DD5472-8C3B-423D-B078-5E3B4DC3F79D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1186,7 +1187,7 @@
   <dimension ref="A1:UP88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1348,23 +1349,23 @@
     <row r="6" spans="1:17" s="12" customFormat="1">
       <c r="A6" s="67"/>
       <c r="B6" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="G6" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>64</v>
-      </c>
       <c r="H6" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1379,23 +1380,23 @@
     <row r="7" spans="1:17" s="12" customFormat="1">
       <c r="A7" s="68"/>
       <c r="B7" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="20" t="s">
-        <v>64</v>
-      </c>
       <c r="H7" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1445,7 +1446,7 @@
         <v>1.3</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>12</v>
@@ -1478,7 +1479,7 @@
         <v>1.4</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>12</v>
@@ -1580,10 +1581,10 @@
         <v>44083</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="2"/>
@@ -1604,13 +1605,13 @@
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="2"/>
@@ -1626,15 +1627,15 @@
     <row r="16" spans="1:17" s="12" customFormat="1">
       <c r="A16" s="67"/>
       <c r="B16" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>42</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -1651,15 +1652,15 @@
     <row r="17" spans="1:562" s="12" customFormat="1">
       <c r="A17" s="68"/>
       <c r="B17" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>44</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -1673,20 +1674,20 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:562" s="12" customFormat="1">
+    <row r="18" spans="1:562" s="12" customFormat="1" ht="30">
       <c r="A18" s="66">
         <v>2.2000000000000002</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>50</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
@@ -1703,12 +1704,12 @@
     <row r="19" spans="1:562" s="12" customFormat="1">
       <c r="A19" s="68"/>
       <c r="B19" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
       <c r="E19" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" s="20">
         <v>43840</v>
@@ -1730,12 +1731,12 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="20">
         <v>43840</v>
@@ -3487,7 +3488,7 @@
         <v>3</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
@@ -4055,7 +4056,7 @@
         <v>3.1</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
@@ -4665,7 +4666,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="48"/>
       <c r="D30" s="48"/>
@@ -4673,7 +4674,7 @@
         <v>43961</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G30" s="48"/>
       <c r="I30" s="44"/>
@@ -5236,7 +5237,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -5804,7 +5805,7 @@
         <v>4.2</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -6372,7 +6373,7 @@
         <v>4.3</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -6395,7 +6396,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
@@ -6418,7 +6419,7 @@
         <v>4.5</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -6498,7 +6499,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
@@ -6506,7 +6507,7 @@
         <v>43992</v>
       </c>
       <c r="F39" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G39" s="25"/>
       <c r="H39" s="25"/>
@@ -6525,7 +6526,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" s="32"/>
       <c r="D40" s="32"/>
@@ -6539,7 +6540,7 @@
         <v>5.2</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
@@ -6629,7 +6630,7 @@
         <v>6</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
@@ -6637,7 +6638,7 @@
         <v>44114</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G46" s="27"/>
       <c r="H46" s="27"/>
@@ -6656,7 +6657,7 @@
         <v>6.1</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
@@ -6679,7 +6680,7 @@
         <v>6.2</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
@@ -6702,7 +6703,7 @@
         <v>6.3</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
@@ -6725,7 +6726,7 @@
         <v>6.4</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
@@ -6824,7 +6825,7 @@
         <v>7</v>
       </c>
       <c r="B55" s="52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C55" s="52"/>
       <c r="D55" s="52"/>
@@ -6847,12 +6848,12 @@
         <v>7.1</v>
       </c>
       <c r="B56" s="55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C56" s="56"/>
       <c r="D56" s="56"/>
       <c r="E56" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F56" s="57">
         <v>43963</v>
@@ -6893,7 +6894,7 @@
         <v>8</v>
       </c>
       <c r="B58" s="60" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="60"/>
       <c r="D58" s="60"/>
@@ -6916,7 +6917,7 @@
         <v>8.1</v>
       </c>
       <c r="B59" s="55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C59" s="56"/>
       <c r="D59" s="56"/>
@@ -6943,7 +6944,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B60" s="55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C60" s="56"/>
       <c r="D60" s="56"/>
@@ -7008,7 +7009,7 @@
         <v>9</v>
       </c>
       <c r="B63" s="62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C63" s="62"/>
       <c r="D63" s="62"/>
@@ -7031,7 +7032,7 @@
         <v>9.1</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
@@ -7058,7 +7059,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
@@ -7085,15 +7086,15 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
       <c r="E66" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G66" s="19"/>
       <c r="H66" s="18"/>
@@ -7112,15 +7113,15 @@
         <v>9.4</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="19"/>
       <c r="E67" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G67" s="19"/>
       <c r="H67" s="18"/>

</xml_diff>